<commit_message>
Correlation finished and dataframe sorting finished
a bunch of new dataframes, that were helpful for the calculation of the correlation, and correlation between humidity and dengue and population density and dengue
</commit_message>
<xml_diff>
--- a/population_data/province_areas.xlsx
+++ b/population_data/province_areas.xlsx
@@ -3,14 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB96A1C-A0D1-4F3E-B820-4B10D533C274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A4CDD4-A1A4-409B-B6BB-6676C2438C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -32,9 +45,6 @@
     <t>Pathum Thani</t>
   </si>
   <si>
-    <t>Phra Nakhon Si Ayutthaya</t>
-  </si>
-  <si>
     <t>Ang Thong</t>
   </si>
   <si>
@@ -173,9 +183,6 @@
     <t>Amnat Charoen</t>
   </si>
   <si>
-    <t>Bueng Kan</t>
-  </si>
-  <si>
     <t>Nong Bua Lam Phu</t>
   </si>
   <si>
@@ -252,6 +259,12 @@
   </si>
   <si>
     <t>2020</t>
+  </si>
+  <si>
+    <t>P.Nakhon S.Ayutthaya</t>
+  </si>
+  <si>
+    <t>Bungkan</t>
   </si>
 </sst>
 </file>
@@ -704,13 +717,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="7" customWidth="1"/>
     <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
@@ -720,12 +733,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5">
         <v>3161.248</v>
@@ -733,7 +746,7 @@
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5">
         <v>968.37199999999996</v>
@@ -749,7 +762,7 @@
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5">
         <v>4305.7460000000001</v>
@@ -757,7 +770,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5">
         <v>10322.885</v>
@@ -765,7 +778,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5">
         <v>5351</v>
@@ -773,7 +786,7 @@
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>2469.7460000000001</v>
@@ -781,7 +794,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5">
         <v>12778.287</v>
@@ -789,7 +802,7 @@
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5">
         <v>6338</v>
@@ -797,7 +810,7 @@
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5">
         <v>20107.057000000001</v>
@@ -805,7 +818,7 @@
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5">
         <v>11678.369000000001</v>
@@ -813,7 +826,7 @@
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5">
         <v>4363</v>
@@ -821,7 +834,7 @@
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" s="5">
         <v>6009.0079999999998</v>
@@ -829,7 +842,7 @@
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="5">
         <v>6946.7460000000001</v>
@@ -837,7 +850,7 @@
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="5">
         <v>8607.49</v>
@@ -845,7 +858,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5">
         <v>19483.148000000001</v>
@@ -853,7 +866,7 @@
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="5">
         <v>10885.991</v>
@@ -861,7 +874,7 @@
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="5">
         <v>4708.5119999999997</v>
@@ -869,7 +882,7 @@
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5">
         <v>12533.960999999999</v>
@@ -877,7 +890,7 @@
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="5">
         <v>4505.8819999999996</v>
@@ -885,7 +898,7 @@
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="5">
         <v>11424.611999999999</v>
@@ -893,7 +906,7 @@
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="5">
         <v>6199.7529999999997</v>
@@ -901,7 +914,7 @@
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="5">
         <v>12681.259</v>
@@ -909,7 +922,7 @@
     </row>
     <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="5">
         <v>5291.683</v>
@@ -917,7 +930,7 @@
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" s="5">
         <v>4339.83</v>
@@ -925,7 +938,7 @@
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="5">
         <v>2122</v>
@@ -933,7 +946,7 @@
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="5">
         <v>2168.3270000000002</v>
@@ -941,7 +954,7 @@
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" s="5">
         <v>5512.6679999999997</v>
@@ -949,7 +962,7 @@
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="5">
         <v>20493.964</v>
@@ -957,7 +970,7 @@
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="5">
         <v>9597.6769999999997</v>
@@ -965,7 +978,7 @@
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5">
         <v>9942.5020000000004</v>
@@ -973,7 +986,7 @@
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5">
         <v>11472.072</v>
@@ -981,7 +994,7 @@
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B34" s="5">
         <v>4475.43</v>
@@ -989,7 +1002,7 @@
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5">
         <v>3859.0859999999998</v>
@@ -997,7 +1010,7 @@
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="5">
         <v>3026.5340000000001</v>
@@ -1013,66 +1026,66 @@
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B38" s="5">
-        <v>1525.856</v>
+        <v>2556.64</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B39" s="5">
-        <v>1940.356</v>
+        <v>1525.856</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B40" s="5">
-        <v>4170.8950000000004</v>
+        <v>1940.356</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B41" s="5">
-        <v>3424.473</v>
+        <v>4170.8950000000004</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B42" s="5">
-        <v>6355.06</v>
+        <v>3424.473</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B43" s="5">
-        <v>12668.415999999999</v>
+        <v>6355.06</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B44" s="5">
-        <v>6225.1379999999999</v>
+        <v>12668.415999999999</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B45" s="5">
-        <v>4531.0129999999999</v>
+        <v>6225.1379999999999</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1080,20 +1093,20 @@
         <v>41</v>
       </c>
       <c r="B46" s="5">
-        <v>10815.853999999999</v>
+        <v>4531.0129999999999</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B47" s="5">
-        <v>2556.64</v>
+        <v>10815.853999999999</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="5">
         <v>6538.598</v>
@@ -1101,7 +1114,7 @@
     </row>
     <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B49" s="5">
         <v>543.03399999999999</v>
@@ -1109,7 +1122,7 @@
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" s="5">
         <v>4762.3620000000001</v>
@@ -1117,7 +1130,7 @@
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B51" s="5">
         <v>6367.62</v>
@@ -1125,7 +1138,7 @@
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B52" s="5">
         <v>3298.0450000000001</v>
@@ -1133,7 +1146,7 @@
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="5">
         <v>5196.4620000000004</v>
@@ -1141,7 +1154,7 @@
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="5">
         <v>3552</v>
@@ -1149,7 +1162,7 @@
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55" s="5">
         <v>8299.4490000000005</v>
@@ -1157,7 +1170,7 @@
     </row>
     <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B56" s="5">
         <v>7195.1379999999999</v>
@@ -1165,7 +1178,7 @@
     </row>
     <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B57" s="5">
         <v>9605.7639999999992</v>
@@ -1181,7 +1194,7 @@
     </row>
     <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59" s="5">
         <v>872.34699999999998</v>
@@ -1189,7 +1202,7 @@
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60" s="5">
         <v>416.70699999999999</v>
@@ -1197,7 +1210,7 @@
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61" s="5">
         <v>3576.4859999999999</v>
@@ -1205,7 +1218,7 @@
     </row>
     <row r="62" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B62" s="5">
         <v>2478.9769999999999</v>
@@ -1213,7 +1226,7 @@
     </row>
     <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B63" s="5">
         <v>8839.9760000000006</v>
@@ -1221,7 +1234,7 @@
     </row>
     <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B64" s="5">
         <v>822.47799999999995</v>
@@ -1229,7 +1242,7 @@
     </row>
     <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B65" s="5">
         <v>7393.8890000000001</v>
@@ -1237,7 +1250,7 @@
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="5">
         <v>6596.0919999999996</v>
@@ -1245,7 +1258,7 @@
     </row>
     <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="5">
         <v>5358.0079999999998</v>
@@ -1253,7 +1266,7 @@
     </row>
     <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B68" s="5">
         <v>12891.468999999999</v>
@@ -1261,7 +1274,7 @@
     </row>
     <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" s="5">
         <v>8124.0559999999996</v>
@@ -1269,7 +1282,7 @@
     </row>
     <row r="70" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B70" s="5">
         <v>16406.650000000001</v>
@@ -1277,7 +1290,7 @@
     </row>
     <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" s="5">
         <v>4917.5190000000002</v>
@@ -1285,7 +1298,7 @@
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72" s="5">
         <v>2819</v>
@@ -1293,7 +1306,7 @@
     </row>
     <row r="73" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B73" s="5">
         <v>15744.85</v>
@@ -1301,7 +1314,7 @@
     </row>
     <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B74" s="5">
         <v>11730.302</v>
@@ -1309,7 +1322,7 @@
     </row>
     <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B75" s="5">
         <v>6730.2460000000001</v>
@@ -1317,7 +1330,7 @@
     </row>
     <row r="76" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="5">
         <v>7838.5919999999996</v>
@@ -1325,7 +1338,7 @@
     </row>
     <row r="77" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B77" s="5">
         <v>4521.0780000000004</v>
@@ -1333,7 +1346,7 @@
     </row>
     <row r="78" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B78" s="6">
         <v>4161.6639999999998</v>
@@ -1343,8 +1356,8 @@
       <c r="A79" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B78">
-    <sortCondition ref="A2:A78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B79">
+    <sortCondition ref="A1:A79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>